<commit_message>
upd nomenclautre of logical block and readme
</commit_message>
<xml_diff>
--- a/code/outputs/dataset_with_ORI.xlsx
+++ b/code/outputs/dataset_with_ORI.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>sentence_uniqueness_ratio</t>
+          <t>logical_block_uniqueness_ratio</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>norm(sentence_uniqueness_ratio)</t>
+          <t>norm(logical_block_uniqueness_ratio)</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -525,7 +525,7 @@
         <v>16.96616637053628</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1103136187042927</v>
+        <v>0.5705319720580332</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -534,13 +534,13 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>0.5198498702541686</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>0.8845690472280845</v>
       </c>
       <c r="M2" t="n">
-        <v>0.6358471059440458</v>
+        <v>0.814017582221236</v>
       </c>
     </row>
     <row r="3">
@@ -568,10 +568,10 @@
         <v>14.63456858789024</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>0.517281553398058</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>0.8076923076923075</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -583,50 +583,93 @@
         <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1455914957876572</v>
+        <v>0.7263652440994914</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>resource--leak_type=parsed.ttl</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>12072</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.3580246913580247</v>
+      </c>
+      <c r="G4" t="n">
+        <v>34.83363761275684</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>rvl_type=parsed.ttl</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B5" t="n">
         <v>6532</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C5" t="n">
         <v>1.041666666666667</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" t="n">
         <v>0.2444444444444444</v>
       </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
         <v>0.5700757575757576</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G5" t="n">
         <v>16.41879241539388</v>
       </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.1999999999999996</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.6420975521940887</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.2347634567233137</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.3403583299518649</v>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.8461538461538459</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.828153093249641</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.9116680167136849</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.807827298459074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>